<commit_message>
risk parameters calc complete
</commit_message>
<xml_diff>
--- a/economic parameters.xlsx
+++ b/economic parameters.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="800" windowWidth="49160" windowHeight="23880" activeTab="3"/>
+    <workbookView xWindow="17280" yWindow="6020" windowWidth="31280" windowHeight="18340" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="179">
   <si>
     <t>Island Country EEZ</t>
   </si>
@@ -474,6 +475,9 @@
     <t>Control of Corruption</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ease of doing buisness </t>
   </si>
   <si>
@@ -513,6 +517,9 @@
     <t>Corruptions Perception Index (http://www.transparency.org/news/feature/corruption_perceptions_index_2016)</t>
   </si>
   <si>
+    <t>FDI Potential</t>
+  </si>
+  <si>
     <t>Inflation Index</t>
   </si>
   <si>
@@ -604,6 +611,45 @@
   </si>
   <si>
     <t>Attitude of Governement</t>
+  </si>
+  <si>
+    <t>FDI</t>
+  </si>
+  <si>
+    <t>Trade as % GDP</t>
+  </si>
+  <si>
+    <t>CPI Growth</t>
+  </si>
+  <si>
+    <t>GDP growth</t>
+  </si>
+  <si>
+    <t>merchandise esports growth rate</t>
+  </si>
+  <si>
+    <t>McGowan and Moeller 2009</t>
+  </si>
+  <si>
+    <t>Substitute Component</t>
+  </si>
+  <si>
+    <t>r value</t>
+  </si>
+  <si>
+    <t>p value</t>
+  </si>
+  <si>
+    <t>Attitude of government</t>
+  </si>
+  <si>
+    <t>FDI net inflows</t>
+  </si>
+  <si>
+    <t>FDI potential*</t>
+  </si>
+  <si>
+    <t>*took max overall ranking value - country overall rank value to invert scores</t>
   </si>
 </sst>
 </file>
@@ -671,7 +717,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,6 +739,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,12 +909,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -897,6 +957,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -991,6 +1052,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1012,9 +1076,59 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1151,7 +1265,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2541,9 +2655,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA3" sqref="AA3:AA30"/>
+      <selection pane="topRight" activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2564,7 +2678,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H1" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -2574,11 +2688,11 @@
       <c r="N1" s="18"/>
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
-      <c r="Q1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
+      <c r="Q1" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:31" ht="120" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2588,89 +2702,89 @@
         <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="O2" s="26" t="s">
         <v>121</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="O2" s="25" t="s">
-        <v>120</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="R2" s="24" t="s">
         <v>129</v>
       </c>
+      <c r="R2" s="25" t="s">
+        <v>130</v>
+      </c>
       <c r="S2" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="U2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA2" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>133</v>
-      </c>
       <c r="AB2" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
@@ -2712,20 +2826,20 @@
       <c r="P3">
         <v>6.2</v>
       </c>
-      <c r="Q3" s="20">
+      <c r="Q3" s="21">
         <v>2</v>
       </c>
-      <c r="R3" s="20">
+      <c r="R3" s="21">
         <v>2</v>
       </c>
-      <c r="S3" s="20">
+      <c r="S3" s="21">
         <v>2</v>
       </c>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
       <c r="V3" s="9"/>
       <c r="AA3" s="9"/>
-      <c r="AC3" s="42">
+      <c r="AC3" s="43">
         <v>21493</v>
       </c>
       <c r="AD3">
@@ -2775,23 +2889,23 @@
       <c r="O4">
         <v>58.04</v>
       </c>
-      <c r="Q4" s="20">
+      <c r="Q4" s="21">
         <v>2</v>
       </c>
-      <c r="R4" s="20">
+      <c r="R4" s="21">
         <v>2</v>
       </c>
-      <c r="S4" s="20">
+      <c r="S4" s="21">
         <v>2</v>
       </c>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
       <c r="V4" s="9"/>
       <c r="Y4">
         <v>126</v>
       </c>
       <c r="AA4" s="9"/>
-      <c r="AC4" s="42">
+      <c r="AC4" s="43">
         <v>24100</v>
       </c>
       <c r="AD4">
@@ -2836,14 +2950,14 @@
         <f>AVERAGE(H5:M5)</f>
         <v>0.85249999999999992</v>
       </c>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
       <c r="V5" s="9"/>
       <c r="AA5" s="9"/>
-      <c r="AC5" s="42">
+      <c r="AC5" s="43">
         <v>25300</v>
       </c>
       <c r="AD5">
@@ -2886,7 +3000,7 @@
       <c r="L6" s="17">
         <v>0.56000000000000005</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="24">
         <v>1.29</v>
       </c>
       <c r="N6" s="16">
@@ -2899,44 +3013,44 @@
       <c r="P6">
         <v>0.3</v>
       </c>
-      <c r="Q6" s="20">
+      <c r="Q6" s="21">
         <v>2</v>
       </c>
-      <c r="R6" s="20">
+      <c r="R6" s="21">
         <v>2</v>
       </c>
-      <c r="S6" s="20">
+      <c r="S6" s="21">
         <v>2</v>
       </c>
-      <c r="T6" s="26">
+      <c r="T6" s="27">
         <v>66</v>
       </c>
-      <c r="U6" s="26">
+      <c r="U6" s="27">
         <f>T6/20</f>
         <v>3.3</v>
       </c>
-      <c r="V6" s="20">
+      <c r="V6" s="21">
         <v>50</v>
       </c>
-      <c r="W6" s="20">
+      <c r="W6" s="21">
         <f>V6/20</f>
         <v>2.5</v>
       </c>
-      <c r="Y6" s="20">
+      <c r="Y6" s="21">
         <v>95</v>
       </c>
-      <c r="Z6" s="20" t="e">
+      <c r="Z6" s="21" t="e">
         <f>#REF!/20</f>
         <v>#REF!</v>
       </c>
-      <c r="AA6" s="20">
+      <c r="AA6" s="21">
         <v>76.099999999999994</v>
       </c>
       <c r="AB6">
         <f>AA6/20</f>
         <v>3.8049999999999997</v>
       </c>
-      <c r="AC6" s="43">
+      <c r="AC6" s="44">
         <v>24600</v>
       </c>
       <c r="AD6">
@@ -2982,7 +3096,7 @@
       <c r="L7" s="17">
         <v>1.05</v>
       </c>
-      <c r="M7" s="23">
+      <c r="M7" s="24">
         <v>1.79</v>
       </c>
       <c r="N7" s="16">
@@ -2995,33 +3109,33 @@
       <c r="P7">
         <v>1.7</v>
       </c>
-      <c r="Q7" s="20">
+      <c r="Q7" s="21">
         <v>1</v>
       </c>
-      <c r="R7" s="20">
+      <c r="R7" s="21">
         <v>2</v>
       </c>
-      <c r="S7" s="20">
+      <c r="S7" s="21">
         <v>3</v>
       </c>
-      <c r="T7" s="26">
+      <c r="T7" s="27">
         <v>61</v>
       </c>
-      <c r="U7" s="26">
+      <c r="U7" s="27">
         <f>T7/20</f>
         <v>3.05</v>
       </c>
-      <c r="V7" s="20">
+      <c r="V7" s="21">
         <v>75</v>
       </c>
-      <c r="W7" s="20">
+      <c r="W7" s="21">
         <f>V7/20</f>
         <v>3.75</v>
       </c>
-      <c r="Y7" s="20">
+      <c r="Y7" s="21">
         <v>97</v>
       </c>
-      <c r="Z7" s="20" t="e">
+      <c r="Z7" s="21" t="e">
         <f>#REF!/20</f>
         <v>#REF!</v>
       </c>
@@ -3032,7 +3146,7 @@
         <f>AA7/20</f>
         <v>4.1850000000000005</v>
       </c>
-      <c r="AC7" s="43">
+      <c r="AC7" s="44">
         <v>17200</v>
       </c>
       <c r="AD7">
@@ -3066,12 +3180,12 @@
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="AC8" s="42">
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="AC8" s="43">
         <v>21500</v>
       </c>
       <c r="AD8">
@@ -3106,26 +3220,26 @@
       <c r="L9" s="15"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
-      <c r="Q9" s="20">
+      <c r="Q9" s="21">
         <v>1</v>
       </c>
-      <c r="R9" s="20">
+      <c r="R9" s="21">
         <v>1</v>
       </c>
-      <c r="S9" s="20">
+      <c r="S9" s="21">
         <v>1</v>
       </c>
-      <c r="T9" s="27"/>
-      <c r="U9" s="26">
+      <c r="T9" s="28"/>
+      <c r="U9" s="27">
         <f>T9/20</f>
         <v>0</v>
       </c>
       <c r="V9" s="9"/>
-      <c r="W9" s="20">
+      <c r="W9" s="21">
         <f>V9/20</f>
         <v>0</v>
       </c>
-      <c r="Z9" s="20" t="e">
+      <c r="Z9" s="21" t="e">
         <f>#REF!/20</f>
         <v>#REF!</v>
       </c>
@@ -3134,7 +3248,7 @@
         <f>AA9/20</f>
         <v>0</v>
       </c>
-      <c r="AC9" s="43">
+      <c r="AC9" s="44">
         <v>42300</v>
       </c>
       <c r="AD9">
@@ -3177,33 +3291,33 @@
       <c r="L10" s="17">
         <v>0.89</v>
       </c>
-      <c r="M10" s="23">
+      <c r="M10" s="24">
         <v>1.03</v>
       </c>
       <c r="N10" s="16">
         <f>AVERAGE(H10:M10)</f>
         <v>0.91833333333333333</v>
       </c>
-      <c r="Q10" s="20">
+      <c r="Q10" s="21">
         <v>1</v>
       </c>
-      <c r="R10" s="20">
+      <c r="R10" s="21">
         <v>1</v>
       </c>
-      <c r="S10" s="20">
+      <c r="S10" s="21">
         <v>1</v>
       </c>
-      <c r="T10" s="27"/>
-      <c r="U10" s="26">
+      <c r="T10" s="28"/>
+      <c r="U10" s="27">
         <f>T10/20</f>
         <v>0</v>
       </c>
       <c r="V10" s="9"/>
-      <c r="W10" s="20">
+      <c r="W10" s="21">
         <f>V10/20</f>
         <v>0</v>
       </c>
-      <c r="Z10" s="20" t="e">
+      <c r="Z10" s="21" t="e">
         <f>#REF!/20</f>
         <v>#REF!</v>
       </c>
@@ -3212,7 +3326,7 @@
         <f>AA10/20</f>
         <v>0</v>
       </c>
-      <c r="AC10" s="43">
+      <c r="AC10" s="44">
         <v>43800</v>
       </c>
       <c r="AD10">
@@ -3255,31 +3369,31 @@
       <c r="L11" s="17">
         <v>-0.62</v>
       </c>
-      <c r="M11" s="23">
+      <c r="M11" s="24">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N11" s="16">
         <f>AVERAGE(H11:M11)</f>
         <v>-0.45666666666666672</v>
       </c>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="27">
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="28">
         <v>47</v>
       </c>
-      <c r="U11" s="26">
+      <c r="U11" s="27">
         <f>T11/20</f>
         <v>2.35</v>
       </c>
       <c r="V11" s="9">
         <v>10</v>
       </c>
-      <c r="W11" s="20">
+      <c r="W11" s="21">
         <f>V11/20</f>
         <v>0.5</v>
       </c>
-      <c r="Z11" s="20" t="e">
+      <c r="Z11" s="21" t="e">
         <f>#REF!/20</f>
         <v>#REF!</v>
       </c>
@@ -3290,7 +3404,7 @@
         <f>AA11/20</f>
         <v>3.3</v>
       </c>
-      <c r="AC11" s="43">
+      <c r="AC11" s="44">
         <v>11600</v>
       </c>
       <c r="AD11">
@@ -3325,26 +3439,26 @@
       <c r="L12" s="15"/>
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
-      <c r="Q12" s="20">
+      <c r="Q12" s="21">
         <v>2</v>
       </c>
-      <c r="R12" s="20">
+      <c r="R12" s="21">
         <v>2</v>
       </c>
-      <c r="S12" s="20">
+      <c r="S12" s="21">
         <v>1</v>
       </c>
-      <c r="T12" s="27"/>
-      <c r="U12" s="26">
+      <c r="T12" s="28"/>
+      <c r="U12" s="27">
         <f>T12/20</f>
         <v>0</v>
       </c>
       <c r="V12" s="9"/>
-      <c r="W12" s="20">
+      <c r="W12" s="21">
         <f>V12/20</f>
         <v>0</v>
       </c>
-      <c r="Z12" s="20" t="e">
+      <c r="Z12" s="21" t="e">
         <f>#REF!/20</f>
         <v>#REF!</v>
       </c>
@@ -3353,7 +3467,7 @@
         <f>AA12/20</f>
         <v>0</v>
       </c>
-      <c r="AC12" s="43">
+      <c r="AC12" s="44">
         <v>15000</v>
       </c>
       <c r="AD12">
@@ -3396,7 +3510,7 @@
       <c r="L13" s="17">
         <v>0.64</v>
       </c>
-      <c r="M13" s="23">
+      <c r="M13" s="24">
         <v>0.62</v>
       </c>
       <c r="N13" s="16">
@@ -3409,27 +3523,27 @@
       <c r="P13">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="27">
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="28">
         <v>59</v>
       </c>
-      <c r="U13" s="26">
+      <c r="U13" s="27">
         <f>T13/20</f>
         <v>2.95</v>
       </c>
       <c r="V13" s="9">
         <v>75</v>
       </c>
-      <c r="W13" s="20">
+      <c r="W13" s="21">
         <f>V13/20</f>
         <v>3.75</v>
       </c>
       <c r="Y13">
         <v>145</v>
       </c>
-      <c r="Z13" s="20" t="e">
+      <c r="Z13" s="21" t="e">
         <f>#REF!/20</f>
         <v>#REF!</v>
       </c>
@@ -3440,7 +3554,7 @@
         <f>AA13/20</f>
         <v>4.4749999999999996</v>
       </c>
-      <c r="AC13" s="43">
+      <c r="AC13" s="44">
         <v>11400</v>
       </c>
       <c r="AD13">
@@ -3483,7 +3597,7 @@
       <c r="L14" s="17">
         <v>-0.46</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="24">
         <v>-0.77</v>
       </c>
       <c r="N14" s="16">
@@ -3496,44 +3610,44 @@
       <c r="P14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q14" s="20">
+      <c r="Q14" s="21">
         <v>3</v>
       </c>
-      <c r="R14" s="20">
+      <c r="R14" s="21">
         <v>2</v>
       </c>
-      <c r="S14" s="20">
+      <c r="S14" s="21">
         <v>4</v>
       </c>
-      <c r="T14" s="26">
+      <c r="T14" s="27">
         <v>31</v>
       </c>
-      <c r="U14" s="26">
+      <c r="U14" s="27">
         <f>T14/20</f>
         <v>1.55</v>
       </c>
-      <c r="V14" s="20">
+      <c r="V14" s="21">
         <v>75</v>
       </c>
-      <c r="W14" s="20">
+      <c r="W14" s="21">
         <f>V14/20</f>
         <v>3.75</v>
       </c>
-      <c r="Y14" s="20">
+      <c r="Y14" s="21">
         <v>79</v>
       </c>
-      <c r="Z14" s="20" t="e">
+      <c r="Z14" s="21" t="e">
         <f>#REF!/20</f>
         <v>#REF!</v>
       </c>
-      <c r="AA14" s="20">
+      <c r="AA14" s="21">
         <v>76.7</v>
       </c>
       <c r="AB14">
         <f>AA14/20</f>
         <v>3.835</v>
       </c>
-      <c r="AC14" s="43">
+      <c r="AC14" s="44">
         <v>15900</v>
       </c>
       <c r="AD14">
@@ -3576,7 +3690,7 @@
       <c r="L15" s="17">
         <v>-0.2</v>
       </c>
-      <c r="M15" s="23">
+      <c r="M15" s="24">
         <v>0.31</v>
       </c>
       <c r="N15" s="16">
@@ -3589,23 +3703,23 @@
       <c r="P15">
         <v>7.3</v>
       </c>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="27">
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="28">
         <v>56</v>
       </c>
-      <c r="U15" s="26">
+      <c r="U15" s="27">
         <f>T15/20</f>
         <v>2.8</v>
       </c>
       <c r="V15" s="9"/>
-      <c r="W15" s="20">
+      <c r="W15" s="21">
         <f>V15/20</f>
         <v>0</v>
       </c>
-      <c r="Y15" s="27"/>
-      <c r="Z15" s="20">
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="21">
         <f>Y15/20</f>
         <v>0</v>
       </c>
@@ -3614,7 +3728,7 @@
         <f>AA15/20</f>
         <v>0</v>
       </c>
-      <c r="AC15" s="43">
+      <c r="AC15" s="44">
         <v>14100</v>
       </c>
       <c r="AD15">
@@ -3647,21 +3761,21 @@
       <c r="L16" s="15"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="26">
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="27">
         <f>T16/20</f>
         <v>0</v>
       </c>
       <c r="V16" s="9"/>
-      <c r="W16" s="20">
+      <c r="W16" s="21">
         <f>V16/20</f>
         <v>0</v>
       </c>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="20">
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="21">
         <f>Y16/20</f>
         <v>0</v>
       </c>
@@ -3670,7 +3784,7 @@
         <f>AA16/20</f>
         <v>0</v>
       </c>
-      <c r="AC16" s="43">
+      <c r="AC16" s="44">
         <v>25479</v>
       </c>
       <c r="AD16">
@@ -3713,7 +3827,7 @@
       <c r="L17" s="17">
         <v>-1.17</v>
       </c>
-      <c r="M17" s="23">
+      <c r="M17" s="24">
         <v>-1.26</v>
       </c>
       <c r="N17" s="16">
@@ -3723,25 +3837,25 @@
       <c r="O17">
         <v>38.659999999999997</v>
       </c>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="27">
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="28">
         <v>20</v>
       </c>
-      <c r="U17" s="26">
+      <c r="U17" s="27">
         <f>T17/20</f>
         <v>1</v>
       </c>
       <c r="V17" s="9"/>
-      <c r="W17" s="20">
+      <c r="W17" s="21">
         <f>V17/20</f>
         <v>0</v>
       </c>
-      <c r="Y17" s="27">
+      <c r="Y17" s="28">
         <v>160</v>
       </c>
-      <c r="Z17" s="20">
+      <c r="Z17" s="21">
         <f>Y17/20</f>
         <v>8</v>
       </c>
@@ -3752,7 +3866,7 @@
         <f>AA17/20</f>
         <v>3.69</v>
       </c>
-      <c r="AC17" s="43">
+      <c r="AC17" s="44">
         <v>1800</v>
       </c>
       <c r="AD17">
@@ -3795,7 +3909,7 @@
       <c r="L18" s="17">
         <v>-0.23</v>
       </c>
-      <c r="M18" s="23">
+      <c r="M18" s="24">
         <v>-0.33</v>
       </c>
       <c r="N18" s="16">
@@ -3808,31 +3922,31 @@
       <c r="P18">
         <v>2.8</v>
       </c>
-      <c r="Q18" s="20">
+      <c r="Q18" s="21">
         <v>2</v>
       </c>
-      <c r="R18" s="20">
+      <c r="R18" s="21">
         <v>3</v>
       </c>
-      <c r="S18" s="20">
+      <c r="S18" s="21">
         <v>4</v>
       </c>
-      <c r="T18" s="27"/>
-      <c r="U18" s="26">
+      <c r="T18" s="28"/>
+      <c r="U18" s="27">
         <f>T18/20</f>
         <v>0</v>
       </c>
-      <c r="V18" s="20">
+      <c r="V18" s="21">
         <v>80</v>
       </c>
-      <c r="W18" s="20">
+      <c r="W18" s="21">
         <f>V18/20</f>
         <v>4</v>
       </c>
-      <c r="Y18" s="26">
+      <c r="Y18" s="27">
         <v>88</v>
       </c>
-      <c r="Z18" s="20">
+      <c r="Z18" s="21">
         <f>Y18/20</f>
         <v>4.4000000000000004</v>
       </c>
@@ -3841,7 +3955,7 @@
         <f>AA18/20</f>
         <v>0</v>
       </c>
-      <c r="AC18" s="43">
+      <c r="AC18" s="44">
         <v>9000</v>
       </c>
       <c r="AD18">
@@ -3880,30 +3994,30 @@
       <c r="L19" s="17">
         <v>-0.02</v>
       </c>
-      <c r="M19" s="23">
+      <c r="M19" s="24">
         <v>1.25</v>
       </c>
       <c r="N19" s="16">
         <f>AVERAGE(H19:M19)</f>
         <v>0.84199999999999997</v>
       </c>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="27">
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="28">
         <v>39</v>
       </c>
-      <c r="U19" s="26">
+      <c r="U19" s="27">
         <f>T19/20</f>
         <v>1.95</v>
       </c>
       <c r="V19" s="9"/>
-      <c r="W19" s="20">
+      <c r="W19" s="21">
         <f>V19/20</f>
         <v>0</v>
       </c>
-      <c r="Y19" s="27"/>
-      <c r="Z19" s="20">
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="21">
         <f>Y19/20</f>
         <v>0</v>
       </c>
@@ -3912,7 +4026,7 @@
         <f>AA19/20</f>
         <v>0</v>
       </c>
-      <c r="AC19" s="43">
+      <c r="AC19" s="44">
         <v>27688</v>
       </c>
       <c r="AD19">
@@ -3947,21 +4061,21 @@
       <c r="L20" s="15"/>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="26">
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="27">
         <f>T20/20</f>
         <v>0</v>
       </c>
       <c r="V20" s="9"/>
-      <c r="W20" s="20">
+      <c r="W20" s="21">
         <f>V20/20</f>
         <v>0</v>
       </c>
-      <c r="Y20" s="27"/>
-      <c r="Z20" s="20">
+      <c r="Y20" s="28"/>
+      <c r="Z20" s="21">
         <f>Y20/20</f>
         <v>0</v>
       </c>
@@ -3970,7 +4084,7 @@
         <f>AA20/20</f>
         <v>0</v>
       </c>
-      <c r="AC20" s="43">
+      <c r="AC20" s="44">
         <v>8500</v>
       </c>
       <c r="AD20">
@@ -4013,7 +4127,7 @@
       <c r="L21" s="17">
         <v>0.78</v>
       </c>
-      <c r="M21" s="23">
+      <c r="M21" s="24">
         <v>0.13</v>
       </c>
       <c r="N21" s="16">
@@ -4026,21 +4140,21 @@
       <c r="P21">
         <v>3.7</v>
       </c>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="26">
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="27">
         <f>T21/20</f>
         <v>0</v>
       </c>
       <c r="V21" s="9"/>
-      <c r="W21" s="20">
+      <c r="W21" s="21">
         <f>V21/20</f>
         <v>0</v>
       </c>
-      <c r="Y21" s="27"/>
-      <c r="Z21" s="20">
+      <c r="Y21" s="28"/>
+      <c r="Z21" s="21">
         <f>Y21/20</f>
         <v>0</v>
       </c>
@@ -4049,7 +4163,7 @@
         <f>AA21/20</f>
         <v>0</v>
       </c>
-      <c r="AC21" s="43">
+      <c r="AC21" s="44">
         <v>37700</v>
       </c>
       <c r="AD21">
@@ -4083,12 +4197,12 @@
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27"/>
-      <c r="AC22" s="42">
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="28"/>
+      <c r="AC22" s="43">
         <v>23600</v>
       </c>
       <c r="AD22">
@@ -4131,7 +4245,7 @@
       <c r="L23" s="17">
         <v>0.35</v>
       </c>
-      <c r="M23" s="23">
+      <c r="M23" s="24">
         <v>0.27</v>
       </c>
       <c r="N23" s="16">
@@ -4141,27 +4255,27 @@
       <c r="O23">
         <v>53.96</v>
       </c>
-      <c r="Q23" s="20">
+      <c r="Q23" s="21">
         <v>2</v>
       </c>
-      <c r="R23" s="20">
+      <c r="R23" s="21">
         <v>2</v>
       </c>
-      <c r="S23" s="20">
+      <c r="S23" s="21">
         <v>1</v>
       </c>
-      <c r="T23" s="27"/>
-      <c r="U23" s="26">
+      <c r="T23" s="28"/>
+      <c r="U23" s="27">
         <f>T23/20</f>
         <v>0</v>
       </c>
       <c r="V23" s="9"/>
-      <c r="W23" s="20">
+      <c r="W23" s="21">
         <f>V23/20</f>
         <v>0</v>
       </c>
-      <c r="Y23" s="27"/>
-      <c r="Z23" s="20">
+      <c r="Y23" s="28"/>
+      <c r="Z23" s="21">
         <f>Y23/20</f>
         <v>0</v>
       </c>
@@ -4170,7 +4284,7 @@
         <f>AA23/20</f>
         <v>0</v>
       </c>
-      <c r="AC23" s="43">
+      <c r="AC23" s="44">
         <v>25500</v>
       </c>
       <c r="AD23">
@@ -4213,7 +4327,7 @@
       <c r="L24" s="17">
         <v>0.62</v>
       </c>
-      <c r="M24" s="23">
+      <c r="M24" s="24">
         <v>0.45</v>
       </c>
       <c r="N24" s="16">
@@ -4223,31 +4337,31 @@
       <c r="O24">
         <v>63.13</v>
       </c>
-      <c r="Q24" s="20">
+      <c r="Q24" s="21">
         <v>1</v>
       </c>
-      <c r="R24" s="20">
+      <c r="R24" s="21">
         <v>2</v>
       </c>
-      <c r="S24" s="20">
+      <c r="S24" s="21">
         <v>2</v>
       </c>
-      <c r="T24" s="26">
+      <c r="T24" s="27">
         <v>60</v>
       </c>
-      <c r="U24" s="26">
+      <c r="U24" s="27">
         <f>T24/20</f>
         <v>3</v>
       </c>
-      <c r="V24" s="20">
+      <c r="V24" s="21">
         <v>65</v>
       </c>
-      <c r="W24" s="20">
+      <c r="W24" s="21">
         <f>V24/20</f>
         <v>3.25</v>
       </c>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="20">
+      <c r="Y24" s="28"/>
+      <c r="Z24" s="21">
         <f>Y24/20</f>
         <v>0</v>
       </c>
@@ -4258,7 +4372,7 @@
         <f>AA24/20</f>
         <v>4.1150000000000002</v>
       </c>
-      <c r="AC24" s="43">
+      <c r="AC24" s="44">
         <v>12000</v>
       </c>
       <c r="AD24">
@@ -4299,27 +4413,27 @@
       <c r="P25">
         <v>6.9</v>
       </c>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
-      <c r="T25" s="27">
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="28">
         <v>60</v>
       </c>
-      <c r="U25" s="26">
+      <c r="U25" s="27">
         <f>T25/20</f>
         <v>3</v>
       </c>
       <c r="V25" s="9">
         <v>75</v>
       </c>
-      <c r="W25" s="20">
+      <c r="W25" s="21">
         <f>V25/20</f>
         <v>3.75</v>
       </c>
-      <c r="Y25" s="27">
+      <c r="Y25" s="28">
         <v>149</v>
       </c>
-      <c r="Z25" s="20">
+      <c r="Z25" s="21">
         <f>Y25/20</f>
         <v>7.45</v>
       </c>
@@ -4330,7 +4444,7 @@
         <f>AA25/20</f>
         <v>4.1450000000000005</v>
       </c>
-      <c r="AC25" s="43">
+      <c r="AC25" s="44">
         <v>11300</v>
       </c>
       <c r="AD25">
@@ -4363,21 +4477,21 @@
       <c r="L26" s="15"/>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="26">
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="27">
         <f>T26/20</f>
         <v>0</v>
       </c>
       <c r="V26" s="9"/>
-      <c r="W26" s="20">
+      <c r="W26" s="21">
         <f>V26/20</f>
         <v>0</v>
       </c>
-      <c r="Y26" s="27"/>
-      <c r="Z26" s="20">
+      <c r="Y26" s="28"/>
+      <c r="Z26" s="21">
         <f>Y26/20</f>
         <v>0</v>
       </c>
@@ -4386,7 +4500,7 @@
         <f>AA26/20</f>
         <v>0</v>
       </c>
-      <c r="AC26" s="43">
+      <c r="AC26" s="44">
         <v>27737</v>
       </c>
       <c r="AD26">
@@ -4419,27 +4533,27 @@
       <c r="L27" s="15"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
-      <c r="Q27" s="20">
+      <c r="Q27" s="21">
         <v>2</v>
       </c>
-      <c r="R27" s="20">
+      <c r="R27" s="21">
         <v>2</v>
       </c>
-      <c r="S27" s="20">
+      <c r="S27" s="21">
         <v>1</v>
       </c>
-      <c r="T27" s="27"/>
-      <c r="U27" s="26">
+      <c r="T27" s="28"/>
+      <c r="U27" s="27">
         <f>T27/20</f>
         <v>0</v>
       </c>
       <c r="V27" s="9"/>
-      <c r="W27" s="20">
+      <c r="W27" s="21">
         <f>V27/20</f>
         <v>0</v>
       </c>
-      <c r="Y27" s="27"/>
-      <c r="Z27" s="20">
+      <c r="Y27" s="28"/>
+      <c r="Z27" s="21">
         <f>Y27/20</f>
         <v>0</v>
       </c>
@@ -4448,7 +4562,7 @@
         <f>AA27/20</f>
         <v>0</v>
       </c>
-      <c r="AC27" s="43">
+      <c r="AC27" s="44">
         <v>19300</v>
       </c>
       <c r="AD27">
@@ -4482,12 +4596,12 @@
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="27"/>
-      <c r="AC28" s="42">
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="28"/>
+      <c r="U28" s="28"/>
+      <c r="AC28" s="43">
         <v>26400</v>
       </c>
       <c r="AD28">
@@ -4518,21 +4632,21 @@
       <c r="L29" s="15"/>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="20"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="26">
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="28"/>
+      <c r="U29" s="27">
         <f>T29/20</f>
         <v>0</v>
       </c>
       <c r="V29" s="9"/>
-      <c r="W29" s="20">
+      <c r="W29" s="21">
         <f>V29/20</f>
         <v>0</v>
       </c>
-      <c r="Y29" s="27"/>
-      <c r="Z29" s="20">
+      <c r="Y29" s="28"/>
+      <c r="Z29" s="21">
         <f>Y29/20</f>
         <v>0</v>
       </c>
@@ -4541,7 +4655,7 @@
         <f>AA29/20</f>
         <v>0</v>
       </c>
-      <c r="AC29" s="43">
+      <c r="AC29" s="44">
         <v>15469</v>
       </c>
       <c r="AD29">
@@ -4596,44 +4710,44 @@
       <c r="P30">
         <v>1.7</v>
       </c>
-      <c r="Q30" s="20">
+      <c r="Q30" s="21">
         <v>2</v>
       </c>
-      <c r="R30" s="20">
+      <c r="R30" s="21">
         <v>2</v>
       </c>
-      <c r="S30" s="20">
+      <c r="S30" s="21">
         <v>2</v>
       </c>
-      <c r="T30" s="26">
+      <c r="T30" s="27">
         <v>35</v>
       </c>
-      <c r="U30" s="26">
+      <c r="U30" s="27">
         <f>T30/20</f>
         <v>1.75</v>
       </c>
-      <c r="V30" s="20">
+      <c r="V30" s="21">
         <v>60</v>
       </c>
-      <c r="W30" s="20">
+      <c r="W30" s="21">
         <f>V30/20</f>
         <v>3</v>
       </c>
-      <c r="Y30" s="26">
+      <c r="Y30" s="27">
         <v>78</v>
       </c>
-      <c r="Z30" s="20">
+      <c r="Z30" s="21">
         <f>Y30/20</f>
         <v>3.9</v>
       </c>
-      <c r="AA30" s="20">
+      <c r="AA30" s="21">
         <v>75.900000000000006</v>
       </c>
       <c r="AB30">
         <f>AA30/20</f>
         <v>3.7950000000000004</v>
       </c>
-      <c r="AC30" s="42">
+      <c r="AC30" s="43">
         <v>31900</v>
       </c>
       <c r="AD30">
@@ -4667,12 +4781,12 @@
       <c r="L31" s="15"/>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="27"/>
-      <c r="AC31" s="42">
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="28"/>
+      <c r="U31" s="28"/>
+      <c r="AC31" s="43">
         <v>29100</v>
       </c>
       <c r="AD31">
@@ -4719,12 +4833,12 @@
         <f>AVERAGE(H32:M32)</f>
         <v>0.93200000000000005</v>
       </c>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="27"/>
-      <c r="U32" s="27"/>
-      <c r="AC32" s="42">
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="28"/>
+      <c r="U32" s="28"/>
+      <c r="AC32" s="43">
         <v>36100</v>
       </c>
       <c r="AD32">
@@ -4733,7 +4847,7 @@
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AC34" s="42">
+      <c r="AC34" s="43">
         <f>MAX(AC3:AC32)</f>
         <v>43800</v>
       </c>
@@ -4749,26 +4863,26 @@
     </row>
     <row r="36" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="U36" s="12" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="V36" s="12" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="W36" s="12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="T37" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="U37" s="29">
+      <c r="T37" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="U37" s="30">
         <v>3.75</v>
       </c>
-      <c r="V37" s="45">
+      <c r="V37" s="46">
         <v>0.35</v>
       </c>
-      <c r="W37" s="30">
+      <c r="W37" s="31">
         <f>U37*V37</f>
         <v>1.3125</v>
       </c>
@@ -4778,154 +4892,154 @@
         <f>CORREL(O3:O27,'[1]Caribbean fuel price'!$C$2:$C$28)</f>
         <v>#N/A</v>
       </c>
-      <c r="T38" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="U38" s="32">
+      <c r="T38" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="U38" s="33">
         <v>1</v>
       </c>
-      <c r="V38" s="46">
+      <c r="V38" s="47">
         <v>0.35</v>
       </c>
-      <c r="W38" s="30">
+      <c r="W38" s="31">
         <f>U38*V38</f>
         <v>0.35</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="T39" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="U39" s="32">
+      <c r="T39" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="U39" s="33">
         <v>3.05</v>
       </c>
-      <c r="V39" s="46">
+      <c r="V39" s="47">
         <v>0.3</v>
       </c>
-      <c r="W39" s="30">
+      <c r="W39" s="31">
         <f>U39*V39</f>
         <v>0.91499999999999992</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="T40" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="U40" s="34"/>
-      <c r="V40" s="47"/>
-      <c r="W40" s="35">
+      <c r="T40" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="U40" s="35"/>
+      <c r="V40" s="48"/>
+      <c r="W40" s="36">
         <f>SUM(W37:W39)</f>
         <v>2.5775000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="T41" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="U41" s="29">
+      <c r="T41" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="U41" s="30">
         <v>1.96</v>
       </c>
-      <c r="V41" s="45">
+      <c r="V41" s="46">
         <v>0.3</v>
       </c>
-      <c r="W41" s="30">
+      <c r="W41" s="31">
         <f>U41*V41</f>
         <v>0.58799999999999997</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="T42" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="U42" s="44">
+      <c r="T42" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="U42" s="45">
         <v>3.5</v>
       </c>
-      <c r="V42" s="36">
+      <c r="V42" s="37">
         <v>0.35</v>
       </c>
-      <c r="W42" s="30">
+      <c r="W42" s="31">
         <f t="shared" ref="W42:W43" si="0">U42*V42</f>
         <v>1.2249999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="T43" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="U43" s="44">
+      <c r="T43" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="U43" s="45">
         <v>3.8</v>
       </c>
-      <c r="V43" s="36">
+      <c r="V43" s="37">
         <v>0.35</v>
       </c>
-      <c r="W43" s="30">
+      <c r="W43" s="31">
         <f t="shared" si="0"/>
         <v>1.3299999999999998</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>149</v>
-      </c>
-      <c r="T44" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="U44" s="34"/>
-      <c r="V44" s="34"/>
-      <c r="W44" s="35">
+        <v>151</v>
+      </c>
+      <c r="T44" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="U44" s="35"/>
+      <c r="V44" s="35"/>
+      <c r="W44" s="36">
         <f>SUM(W41:W43)</f>
         <v>3.1429999999999998</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="T45" s="40"/>
-      <c r="U45" s="41" t="s">
-        <v>147</v>
-      </c>
-      <c r="V45" s="41" t="s">
+      <c r="T45" s="41"/>
+      <c r="U45" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="V45" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="W45" s="30"/>
+      <c r="W45" s="31"/>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="T46" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="U46" s="32">
+      <c r="T46" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="U46" s="33">
         <v>0.6</v>
       </c>
-      <c r="V46" s="32">
+      <c r="V46" s="33">
         <f>W40</f>
         <v>2.5775000000000001</v>
       </c>
-      <c r="W46" s="33">
+      <c r="W46" s="34">
         <f>U46*V46</f>
         <v>1.5465</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="T47" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="U47" s="32">
+      <c r="T47" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="U47" s="33">
         <v>0.4</v>
       </c>
-      <c r="V47" s="32">
+      <c r="V47" s="33">
         <f>W44</f>
         <v>3.1429999999999998</v>
       </c>
-      <c r="W47" s="33">
+      <c r="W47" s="34">
         <f>U47*V47</f>
         <v>1.2572000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="T48" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="U48" s="34"/>
-      <c r="V48" s="34"/>
-      <c r="W48" s="48">
+      <c r="T48" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="U48" s="35"/>
+      <c r="V48" s="35"/>
+      <c r="W48" s="49">
         <f>SUM(W46:W47)</f>
         <v>2.8037000000000001</v>
       </c>
@@ -4985,771 +5099,1412 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J53"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:R65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="49" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.5" customWidth="1"/>
+    <col min="10" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C3" s="49"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="50"/>
     </row>
     <row r="4" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="49"/>
-      <c r="D4" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="63" t="s">
+      <c r="C4" s="50"/>
+      <c r="D4" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="I4" s="50"/>
+    </row>
+    <row r="5" spans="3:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="C5" s="50"/>
+      <c r="D5" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>160</v>
+      </c>
+      <c r="F5" s="57"/>
+      <c r="G5" s="56">
+        <v>0.35</v>
+      </c>
+      <c r="H5" s="57"/>
+      <c r="I5" s="50"/>
+    </row>
+    <row r="6" spans="3:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="C6" s="50"/>
+      <c r="D6" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="F6" s="50"/>
+      <c r="G6" s="51">
+        <v>0.35</v>
+      </c>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C7" s="50"/>
+      <c r="D7" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" s="50"/>
+      <c r="G7" s="51">
+        <v>0.3</v>
+      </c>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C8" s="50"/>
+      <c r="D8" s="59" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="59"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="50"/>
+    </row>
+    <row r="9" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="50"/>
+      <c r="D9" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="67"/>
+      <c r="F9" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="I9" s="50"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C10" s="50"/>
+      <c r="D10" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="F10" s="57"/>
+      <c r="G10" s="56">
+        <v>0.3</v>
+      </c>
+      <c r="H10" s="57"/>
+      <c r="I10" s="50"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C11" s="50"/>
+      <c r="D11" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="E11" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="F11" s="53"/>
+      <c r="G11" s="52">
+        <v>0.35</v>
+      </c>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+    </row>
+    <row r="12" spans="3:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="C12" s="50"/>
+      <c r="D12" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="H4" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="I4" s="49"/>
-    </row>
-    <row r="5" spans="3:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="C5" s="49"/>
-      <c r="D5" s="55" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="67" t="s">
+      <c r="E12" s="69" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="53"/>
+      <c r="G12" s="52">
+        <v>0.35</v>
+      </c>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="50"/>
+      <c r="D13" s="59" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="59"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="50"/>
+    </row>
+    <row r="14" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="50"/>
+      <c r="D14" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="66"/>
+      <c r="F14" s="65" t="s">
+        <v>149</v>
+      </c>
+      <c r="G14" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="58" t="s">
+        <v>157</v>
+      </c>
+      <c r="I14" s="50"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C15" s="50"/>
+      <c r="D15" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="60"/>
+      <c r="F15" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="50"/>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C16" s="50"/>
+      <c r="D16" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="52"/>
+      <c r="F16" s="50">
+        <v>0.4</v>
+      </c>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C17" s="50"/>
+      <c r="D17" s="64" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="64"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+    </row>
+    <row r="22" spans="3:18" ht="30" x14ac:dyDescent="0.2">
+      <c r="D22" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="90" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="73" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="78" t="s">
+        <v>143</v>
+      </c>
+      <c r="H22" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" s="82" t="s">
+        <v>177</v>
+      </c>
+      <c r="J22" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="K22" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="L22" s="73" t="s">
+        <v>115</v>
+      </c>
+      <c r="M22" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="N22" s="86" t="s">
+        <v>166</v>
+      </c>
+      <c r="O22" t="s">
+        <v>167</v>
+      </c>
+      <c r="P22" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>169</v>
+      </c>
+      <c r="R22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D23" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="91"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="71">
+        <v>21493</v>
+      </c>
+      <c r="I23" s="83"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="89">
+        <v>0.89</v>
+      </c>
+      <c r="L23" s="76">
+        <v>0.92</v>
+      </c>
+      <c r="M23" s="81">
+        <v>1.25</v>
+      </c>
+      <c r="N23" s="84">
+        <v>85.45</v>
+      </c>
+      <c r="O23">
+        <v>-13.29</v>
+      </c>
+      <c r="P23">
+        <v>-1.86</v>
+      </c>
+      <c r="Q23">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D24" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="91"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="71">
+        <v>24100</v>
+      </c>
+      <c r="I24" s="83">
+        <v>31</v>
+      </c>
+      <c r="J24" s="52"/>
+      <c r="K24" s="89">
+        <v>0.53</v>
+      </c>
+      <c r="L24" s="76">
+        <v>0.77</v>
+      </c>
+      <c r="M24" s="81">
+        <v>0.67</v>
+      </c>
+      <c r="N24" s="84">
+        <v>154.06</v>
+      </c>
+      <c r="O24">
+        <v>-14.83</v>
+      </c>
+      <c r="P24">
+        <v>0.72</v>
+      </c>
+      <c r="Q24">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D25" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="91"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="71">
+        <v>25300</v>
+      </c>
+      <c r="I25" s="83"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="89">
+        <v>0.9</v>
+      </c>
+      <c r="L25" s="76">
+        <v>0.92</v>
+      </c>
+      <c r="M25" s="81"/>
+      <c r="N25" s="84">
+        <v>-22.57</v>
+      </c>
+      <c r="O25">
+        <v>17.29</v>
+      </c>
+      <c r="P25">
+        <v>0.48</v>
+      </c>
+      <c r="Q25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D26" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="91">
+        <v>50</v>
+      </c>
+      <c r="F26" s="74"/>
+      <c r="G26" s="79">
+        <v>66</v>
+      </c>
+      <c r="H26" s="72">
+        <v>24600</v>
+      </c>
+      <c r="I26" s="83">
+        <v>82</v>
+      </c>
+      <c r="J26" s="52">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="K26" s="89">
+        <v>0.25</v>
+      </c>
+      <c r="L26" s="76">
+        <v>0.8</v>
+      </c>
+      <c r="M26" s="81">
+        <v>1.29</v>
+      </c>
+      <c r="N26" s="84">
+        <v>384.91</v>
+      </c>
+      <c r="O26">
+        <v>-8.57</v>
+      </c>
+      <c r="P26">
+        <v>1.86</v>
+      </c>
+      <c r="Q26">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D27" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="91">
+        <v>75</v>
+      </c>
+      <c r="F27" s="74"/>
+      <c r="G27" s="79">
+        <v>61</v>
+      </c>
+      <c r="H27" s="72">
+        <v>17200</v>
+      </c>
+      <c r="I27" s="83">
+        <v>80</v>
+      </c>
+      <c r="J27" s="52">
+        <v>83.7</v>
+      </c>
+      <c r="K27" s="89">
+        <v>0.51</v>
+      </c>
+      <c r="L27" s="76">
+        <v>1.32</v>
+      </c>
+      <c r="M27" s="81">
+        <v>1.79</v>
+      </c>
+      <c r="N27" s="84">
+        <v>254.52</v>
+      </c>
+      <c r="O27">
+        <v>-6.74</v>
+      </c>
+      <c r="P27">
+        <v>-1.2</v>
+      </c>
+      <c r="Q27">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D28" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="92"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="71">
+        <v>21500</v>
+      </c>
+      <c r="I28" s="83"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="77"/>
+      <c r="M28" s="81"/>
+      <c r="N28" s="84"/>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D29" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="91"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="72">
+        <v>42300</v>
+      </c>
+      <c r="I29" s="83"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="76"/>
+      <c r="M29" s="81"/>
+      <c r="N29" s="84">
+        <v>51605</v>
+      </c>
+      <c r="P29">
+        <v>0.84</v>
+      </c>
+      <c r="Q29">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D30" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="91"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="72">
+        <v>43800</v>
+      </c>
+      <c r="I30" s="83"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="89">
+        <v>0.82</v>
+      </c>
+      <c r="L30" s="76">
+        <v>1.19</v>
+      </c>
+      <c r="M30" s="81">
+        <v>1.03</v>
+      </c>
+      <c r="N30" s="84">
+        <v>18987.38</v>
+      </c>
+      <c r="P30">
+        <v>-2.93</v>
+      </c>
+      <c r="Q30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D31" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="91">
+        <v>10</v>
+      </c>
+      <c r="F31" s="74"/>
+      <c r="G31" s="79">
+        <v>47</v>
+      </c>
+      <c r="H31" s="72">
+        <v>11600</v>
+      </c>
+      <c r="I31" s="83"/>
+      <c r="J31" s="52">
+        <v>66</v>
+      </c>
+      <c r="K31" s="89">
+        <v>-1.25</v>
+      </c>
+      <c r="L31" s="76">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="M31" s="81">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N31" s="84"/>
+      <c r="O31">
+        <v>3.03</v>
+      </c>
+      <c r="P31">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="Q31">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="D32" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="91"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="72">
+        <v>15000</v>
+      </c>
+      <c r="I32" s="83"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="76"/>
+      <c r="M32" s="81"/>
+      <c r="N32" s="84">
+        <v>175.14</v>
+      </c>
+      <c r="O32">
+        <v>-1761</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="R32">
+        <v>-13.8</v>
+      </c>
+    </row>
+    <row r="33" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D33" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="91">
+        <v>75</v>
+      </c>
+      <c r="F33" s="74"/>
+      <c r="G33" s="79">
+        <v>59</v>
+      </c>
+      <c r="H33" s="72">
+        <v>11400</v>
+      </c>
+      <c r="I33" s="83">
+        <v>32</v>
+      </c>
+      <c r="J33" s="52">
+        <v>89.5</v>
+      </c>
+      <c r="K33" s="89">
+        <v>0.26</v>
+      </c>
+      <c r="L33" s="76">
+        <v>1.19</v>
+      </c>
+      <c r="M33" s="81">
+        <v>0.62</v>
+      </c>
+      <c r="N33" s="84">
+        <v>35.96</v>
+      </c>
+      <c r="O33">
+        <v>-14.4</v>
+      </c>
+      <c r="P33">
+        <v>-1.48</v>
+      </c>
+      <c r="Q33">
+        <v>-1.8</v>
+      </c>
+      <c r="R33">
+        <v>-16.100000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D34" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="91">
+        <v>75</v>
+      </c>
+      <c r="F34" s="74"/>
+      <c r="G34" s="79">
+        <v>31</v>
+      </c>
+      <c r="H34" s="72">
+        <v>15900</v>
+      </c>
+      <c r="I34" s="83">
+        <v>98</v>
+      </c>
+      <c r="J34" s="52">
+        <v>76.7</v>
+      </c>
+      <c r="K34" s="89">
+        <v>-0.04</v>
+      </c>
+      <c r="L34" s="76">
+        <v>0.17</v>
+      </c>
+      <c r="M34" s="81">
+        <v>-0.77</v>
+      </c>
+      <c r="N34" s="84">
+        <v>2221.5</v>
+      </c>
+      <c r="O34">
+        <v>-4.3499999999999996</v>
+      </c>
+      <c r="P34">
+        <v>0.84</v>
+      </c>
+      <c r="Q34">
+        <v>7</v>
+      </c>
+      <c r="R34">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="35" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D35" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="91"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="79">
+        <v>56</v>
+      </c>
+      <c r="H35" s="72">
+        <v>14100</v>
+      </c>
+      <c r="I35" s="84"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="89">
+        <v>0.01</v>
+      </c>
+      <c r="L35" s="76">
+        <v>0.81</v>
+      </c>
+      <c r="M35" s="81">
+        <v>0.31</v>
+      </c>
+      <c r="N35" s="84">
+        <v>60.67</v>
+      </c>
+      <c r="O35">
+        <v>-16.170000000000002</v>
+      </c>
+      <c r="P35">
+        <v>-1</v>
+      </c>
+      <c r="Q35">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R35">
+        <v>-8.6</v>
+      </c>
+    </row>
+    <row r="36" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D36" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="91"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="72">
+        <v>25479</v>
+      </c>
+      <c r="I36" s="84"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="81"/>
+      <c r="N36" s="84"/>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D37" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="91"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="79">
+        <v>20</v>
+      </c>
+      <c r="H37" s="72">
+        <v>1800</v>
+      </c>
+      <c r="I37" s="84">
+        <v>17</v>
+      </c>
+      <c r="J37" s="52">
+        <v>73.8</v>
+      </c>
+      <c r="K37" s="89">
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="L37" s="76">
+        <v>-0.73</v>
+      </c>
+      <c r="M37" s="81">
+        <v>-1.26</v>
+      </c>
+      <c r="N37" s="84">
+        <v>104.2</v>
+      </c>
+      <c r="O37">
+        <v>-31.67</v>
+      </c>
+      <c r="P37">
+        <v>9.02</v>
+      </c>
+      <c r="Q37">
+        <v>1.2</v>
+      </c>
+      <c r="R37">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D38" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="91">
+        <v>80</v>
+      </c>
+      <c r="F38" s="74"/>
+      <c r="G38" s="79"/>
+      <c r="H38" s="72">
+        <v>9000</v>
+      </c>
+      <c r="I38" s="84">
+        <v>89</v>
+      </c>
+      <c r="J38" s="52"/>
+      <c r="K38" s="89">
+        <v>0.11</v>
+      </c>
+      <c r="L38" s="76">
+        <v>0.09</v>
+      </c>
+      <c r="M38" s="81">
+        <v>-0.33</v>
+      </c>
+      <c r="N38" s="84">
+        <v>794.48</v>
+      </c>
+      <c r="O38">
+        <v>-16.989999999999998</v>
+      </c>
+      <c r="P38">
+        <v>3.68</v>
+      </c>
+      <c r="Q38">
+        <v>0.8</v>
+      </c>
+      <c r="R38">
+        <v>-13.1</v>
+      </c>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D39" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="91"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="79">
+        <v>39</v>
+      </c>
+      <c r="H39" s="72">
+        <v>27688</v>
+      </c>
+      <c r="I39" s="84"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="89">
+        <v>1.25</v>
+      </c>
+      <c r="L39" s="76">
+        <v>1.01</v>
+      </c>
+      <c r="M39" s="81">
+        <v>1.25</v>
+      </c>
+      <c r="N39" s="84"/>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D40" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="91"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="79"/>
+      <c r="H40" s="72">
+        <v>8500</v>
+      </c>
+      <c r="I40" s="84"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="89"/>
+      <c r="L40" s="76"/>
+      <c r="M40" s="81"/>
+      <c r="N40" s="84">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="O40">
+        <v>-52.23</v>
+      </c>
+      <c r="P40">
+        <v>-1.18</v>
+      </c>
+      <c r="Q40">
+        <v>2</v>
+      </c>
+      <c r="R40">
+        <v>-11.8</v>
+      </c>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D41" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="91"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="72">
+        <v>37700</v>
+      </c>
+      <c r="I41" s="84"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="89">
+        <v>0.98</v>
+      </c>
+      <c r="L41" s="76">
+        <v>0.84</v>
+      </c>
+      <c r="M41" s="81">
+        <v>0.13</v>
+      </c>
+      <c r="N41" s="84">
+        <v>78.16</v>
+      </c>
+    </row>
+    <row r="42" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D42" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="92"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="79"/>
+      <c r="H42" s="71">
+        <v>23600</v>
+      </c>
+      <c r="I42" s="83"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="89"/>
+      <c r="L42" s="77"/>
+      <c r="M42" s="81"/>
+      <c r="N42" s="84"/>
+    </row>
+    <row r="43" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D43" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="91"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="79"/>
+      <c r="H43" s="72">
+        <v>25500</v>
+      </c>
+      <c r="I43" s="84"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="89">
+        <v>0.17</v>
+      </c>
+      <c r="L43" s="76">
+        <v>0.67</v>
+      </c>
+      <c r="M43" s="81">
+        <v>0.27</v>
+      </c>
+      <c r="N43" s="84">
+        <v>75.67</v>
+      </c>
+      <c r="O43">
+        <v>-9.81</v>
+      </c>
+      <c r="P43">
+        <v>-1.72</v>
+      </c>
+      <c r="Q43">
+        <v>3.8</v>
+      </c>
+      <c r="R43">
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="44" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D44" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="91">
+        <v>65</v>
+      </c>
+      <c r="F44" s="74"/>
+      <c r="G44" s="79">
+        <v>60</v>
+      </c>
+      <c r="H44" s="72">
+        <v>12000</v>
+      </c>
+      <c r="I44" s="84"/>
+      <c r="J44" s="52">
+        <v>82.3</v>
+      </c>
+      <c r="K44" s="89">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L44" s="76">
+        <v>0.86</v>
+      </c>
+      <c r="M44" s="81">
+        <v>0.45</v>
+      </c>
+      <c r="N44" s="84">
+        <v>95.03</v>
+      </c>
+      <c r="O44">
+        <v>-1.37</v>
+      </c>
+      <c r="P44">
+        <v>-0.26</v>
+      </c>
+      <c r="Q44">
+        <v>2.4</v>
+      </c>
+      <c r="R44">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="45" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D45" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="91">
+        <v>75</v>
+      </c>
+      <c r="F45" s="74"/>
+      <c r="G45" s="79">
+        <v>60</v>
+      </c>
+      <c r="H45" s="72">
+        <v>11300</v>
+      </c>
+      <c r="I45" s="84">
+        <v>28</v>
+      </c>
+      <c r="J45" s="52">
+        <v>82.9</v>
+      </c>
+      <c r="K45" s="89"/>
+      <c r="L45" s="76"/>
+      <c r="M45" s="81"/>
+      <c r="N45" s="84">
+        <v>120.74</v>
+      </c>
+      <c r="O45">
+        <v>-30.65</v>
+      </c>
+      <c r="P45">
+        <v>-1.73</v>
+      </c>
+      <c r="Q45">
+        <v>1.6</v>
+      </c>
+      <c r="R45">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="46" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D46" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" s="91"/>
+      <c r="F46" s="74"/>
+      <c r="G46" s="79"/>
+      <c r="H46" s="72">
+        <v>27737</v>
+      </c>
+      <c r="I46" s="84"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="89"/>
+      <c r="L46" s="76"/>
+      <c r="M46" s="81"/>
+      <c r="N46" s="84"/>
+    </row>
+    <row r="47" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D47" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="91"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="79"/>
+      <c r="H47" s="72">
+        <v>19300</v>
+      </c>
+      <c r="I47" s="84"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="89"/>
+      <c r="L47" s="76"/>
+      <c r="M47" s="81"/>
+      <c r="N47" s="84"/>
+      <c r="O47">
+        <v>0.86</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>1.7</v>
+      </c>
+      <c r="R47">
+        <v>-2.6</v>
+      </c>
+    </row>
+    <row r="48" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D48" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="E48" s="92"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="79"/>
+      <c r="H48" s="71">
+        <v>26400</v>
+      </c>
+      <c r="I48" s="83"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="89"/>
+      <c r="L48" s="77"/>
+      <c r="M48" s="81"/>
+      <c r="N48" s="84"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D49" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="91"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="79"/>
+      <c r="H49" s="72">
+        <v>15469</v>
+      </c>
+      <c r="I49" s="84"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="89"/>
+      <c r="L49" s="76"/>
+      <c r="M49" s="81"/>
+      <c r="N49" s="84">
+        <v>10.76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D50" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" s="91">
+        <v>60</v>
+      </c>
+      <c r="F50" s="74"/>
+      <c r="G50" s="79">
+        <v>35</v>
+      </c>
+      <c r="H50" s="71">
+        <v>31900</v>
+      </c>
+      <c r="I50" s="84">
+        <v>99</v>
+      </c>
+      <c r="J50" s="52">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="K50" s="89">
+        <v>0.15</v>
+      </c>
+      <c r="L50" s="76">
+        <v>0.27</v>
+      </c>
+      <c r="M50" s="81">
+        <v>-0.54</v>
+      </c>
+      <c r="N50" s="84">
+        <v>1618.61</v>
+      </c>
+      <c r="O50">
+        <v>24.83</v>
+      </c>
+      <c r="P50">
+        <v>4.66</v>
+      </c>
+      <c r="Q50">
+        <v>-0.04</v>
+      </c>
+      <c r="R50">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D51" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="92"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="79"/>
+      <c r="H51" s="71">
+        <v>29100</v>
+      </c>
+      <c r="I51" s="85"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="89"/>
+      <c r="L51" s="77"/>
+      <c r="M51" s="81"/>
+      <c r="N51" s="84"/>
+      <c r="P51">
+        <v>-0.31</v>
+      </c>
+      <c r="Q51">
+        <v>2</v>
+      </c>
+      <c r="R51">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D52" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="92"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="79"/>
+      <c r="H52" s="71">
+        <v>36100</v>
+      </c>
+      <c r="I52" s="85"/>
+      <c r="J52" s="50"/>
+      <c r="K52" s="89">
+        <v>0.53</v>
+      </c>
+      <c r="L52" s="77">
+        <v>1.32</v>
+      </c>
+      <c r="M52" s="81">
+        <v>0.67</v>
+      </c>
+      <c r="N52" s="87"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="80"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="85"/>
+      <c r="J53" s="50"/>
+      <c r="K53" s="33"/>
+      <c r="N53" s="70"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F54" s="75"/>
+      <c r="G54" s="20"/>
+      <c r="I54" s="15"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D59" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="E59" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="F59" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="55">
-        <v>0.35</v>
-      </c>
-      <c r="H5" s="56"/>
-      <c r="I5" s="49"/>
-    </row>
-    <row r="6" spans="3:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="C6" s="49"/>
-      <c r="D6" s="50" t="s">
-        <v>140</v>
-      </c>
-      <c r="E6" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="50">
-        <v>0.35</v>
-      </c>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C7" s="49"/>
-      <c r="D7" s="50" t="s">
-        <v>141</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>159</v>
-      </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="50">
-        <v>0.3</v>
-      </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C8" s="49"/>
-      <c r="D8" s="58" t="s">
+      <c r="G59" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="H59" s="63" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D60" s="57" t="s">
+        <v>175</v>
+      </c>
+      <c r="E60" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="F60" s="57"/>
+      <c r="G60" s="56">
+        <v>0.85</v>
+      </c>
+      <c r="H60" s="56">
+        <v>7.2500000000000004E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D61" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="58"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="49"/>
-    </row>
-    <row r="9" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="49"/>
-      <c r="D9" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="E9" s="65"/>
-      <c r="F9" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="G9" s="61" t="s">
+      <c r="E61" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="F61" s="50"/>
+      <c r="G61" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="H61" s="51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D62" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="E62" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="F62" s="50"/>
+      <c r="G62" s="51">
+        <v>0.79</v>
+      </c>
+      <c r="H62" s="51">
+        <v>2.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D63" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="E63" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" s="50"/>
+      <c r="G63" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="H63" s="51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D64" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="E64" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="F64" s="50"/>
+      <c r="G64" s="51">
+        <v>-0.77</v>
+      </c>
+      <c r="H64" s="51">
+        <v>1.6500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D65" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="I9" s="49"/>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C10" s="49"/>
-      <c r="D10" s="59" t="s">
-        <v>122</v>
-      </c>
-      <c r="E10" s="59" t="s">
-        <v>160</v>
-      </c>
-      <c r="F10" s="56"/>
-      <c r="G10" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="H10" s="56"/>
-      <c r="I10" s="49"/>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C11" s="49"/>
-      <c r="D11" s="51" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="51" t="s">
-        <v>161</v>
-      </c>
-      <c r="F11" s="52"/>
-      <c r="G11" s="51">
-        <v>0.35</v>
-      </c>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-    </row>
-    <row r="12" spans="3:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="C12" s="49"/>
-      <c r="D12" s="51" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12" s="67" t="s">
-        <v>162</v>
-      </c>
-      <c r="F12" s="52"/>
-      <c r="G12" s="51">
-        <v>0.35</v>
-      </c>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C13" s="49"/>
-      <c r="D13" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" s="58"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="49"/>
-    </row>
-    <row r="14" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="49"/>
-      <c r="D14" s="64" t="s">
-        <v>153</v>
-      </c>
-      <c r="E14" s="64"/>
-      <c r="F14" s="63" t="s">
-        <v>147</v>
-      </c>
-      <c r="G14" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="57" t="s">
-        <v>155</v>
-      </c>
-      <c r="I14" s="49"/>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C15" s="49"/>
-      <c r="D15" s="59" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="56">
-        <v>0.6</v>
-      </c>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="49"/>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C16" s="49"/>
-      <c r="D16" s="51" t="s">
-        <v>150</v>
-      </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="49">
-        <v>0.4</v>
-      </c>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C17" s="49"/>
-      <c r="D17" s="62" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D22" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" s="53" t="s">
-        <v>163</v>
-      </c>
-      <c r="F22" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="G22" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="H22" s="53" t="s">
-        <v>122</v>
-      </c>
-      <c r="I22" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="J22" s="53" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D23" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="51"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="69">
-        <v>21493</v>
-      </c>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D24" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" s="51"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="69">
-        <v>24100</v>
-      </c>
-      <c r="I24" s="51">
-        <v>126</v>
-      </c>
-      <c r="J24" s="51"/>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D25" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="51"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="69">
-        <v>25300</v>
-      </c>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-    </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D26" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="51">
-        <v>50</v>
-      </c>
-      <c r="F26" s="49"/>
-      <c r="G26" s="68">
-        <v>66</v>
-      </c>
-      <c r="H26" s="70">
-        <v>24600</v>
-      </c>
-      <c r="I26" s="51">
-        <v>95</v>
-      </c>
-      <c r="J26" s="51">
-        <v>76.099999999999994</v>
-      </c>
-    </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D27" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="51">
-        <v>75</v>
-      </c>
-      <c r="F27" s="49"/>
-      <c r="G27" s="68">
-        <v>61</v>
-      </c>
-      <c r="H27" s="70">
-        <v>17200</v>
-      </c>
-      <c r="I27" s="51">
-        <v>97</v>
-      </c>
-      <c r="J27" s="51">
-        <v>83.7</v>
-      </c>
-    </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D28" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="52"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="69">
-        <v>21500</v>
-      </c>
-      <c r="I28" s="51"/>
-      <c r="J28" s="52"/>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D29" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="51"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="70">
-        <v>42300</v>
-      </c>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D30" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="51"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="70">
-        <v>43800</v>
-      </c>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D31" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="51">
-        <v>10</v>
-      </c>
-      <c r="F31" s="49"/>
-      <c r="G31" s="68">
-        <v>47</v>
-      </c>
-      <c r="H31" s="70">
-        <v>11600</v>
-      </c>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D32" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="51"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="70">
-        <v>15000</v>
-      </c>
-      <c r="I32" s="51"/>
-      <c r="J32" s="51"/>
-    </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D33" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="51">
-        <v>75</v>
-      </c>
-      <c r="F33" s="49"/>
-      <c r="G33" s="68">
-        <v>59</v>
-      </c>
-      <c r="H33" s="70">
-        <v>11400</v>
-      </c>
-      <c r="I33" s="51">
-        <v>145</v>
-      </c>
-      <c r="J33" s="51">
-        <v>89.5</v>
-      </c>
-    </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D34" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="51">
-        <v>75</v>
-      </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="68">
-        <v>31</v>
-      </c>
-      <c r="H34" s="70">
-        <v>15900</v>
-      </c>
-      <c r="I34" s="51">
-        <v>79</v>
-      </c>
-      <c r="J34" s="51">
-        <v>76.7</v>
-      </c>
-    </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D35" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="51"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="68">
-        <v>56</v>
-      </c>
-      <c r="H35" s="70">
-        <v>14100</v>
-      </c>
-      <c r="I35" s="68"/>
-      <c r="J35" s="51"/>
-    </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D36" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="51"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="70">
-        <v>25479</v>
-      </c>
-      <c r="I36" s="68"/>
-      <c r="J36" s="51"/>
-    </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D37" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="51"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="68">
-        <v>20</v>
-      </c>
-      <c r="H37" s="70">
-        <v>1800</v>
-      </c>
-      <c r="I37" s="68">
-        <v>160</v>
-      </c>
-      <c r="J37" s="51">
-        <v>73.8</v>
-      </c>
-    </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D38" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="51">
-        <v>80</v>
-      </c>
-      <c r="F38" s="49"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="70">
-        <v>9000</v>
-      </c>
-      <c r="I38" s="68">
-        <v>88</v>
-      </c>
-      <c r="J38" s="51"/>
-    </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D39" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="51"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="68">
-        <v>39</v>
-      </c>
-      <c r="H39" s="70">
-        <v>27688</v>
-      </c>
-      <c r="I39" s="68"/>
-      <c r="J39" s="51"/>
-    </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D40" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="51"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="70">
-        <v>8500</v>
-      </c>
-      <c r="I40" s="68"/>
-      <c r="J40" s="51"/>
-    </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D41" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" s="51"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="70">
-        <v>37700</v>
-      </c>
-      <c r="I41" s="68"/>
-      <c r="J41" s="51"/>
-    </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D42" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="52"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="69">
-        <v>23600</v>
-      </c>
-      <c r="I42" s="51"/>
-      <c r="J42" s="52"/>
-    </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D43" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="51"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="70">
-        <v>25500</v>
-      </c>
-      <c r="I43" s="68"/>
-      <c r="J43" s="51"/>
-    </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D44" s="49" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="51">
-        <v>65</v>
-      </c>
-      <c r="F44" s="49"/>
-      <c r="G44" s="68">
-        <v>60</v>
-      </c>
-      <c r="H44" s="70">
-        <v>12000</v>
-      </c>
-      <c r="I44" s="68"/>
-      <c r="J44" s="51">
-        <v>82.3</v>
-      </c>
-    </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D45" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="51">
-        <v>75</v>
-      </c>
-      <c r="F45" s="49"/>
-      <c r="G45" s="68">
-        <v>60</v>
-      </c>
-      <c r="H45" s="70">
-        <v>11300</v>
-      </c>
-      <c r="I45" s="68">
-        <v>149</v>
-      </c>
-      <c r="J45" s="51">
-        <v>82.9</v>
-      </c>
-    </row>
-    <row r="46" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D46" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="E46" s="51"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="68"/>
-      <c r="H46" s="70">
-        <v>27737</v>
-      </c>
-      <c r="I46" s="68"/>
-      <c r="J46" s="51"/>
-    </row>
-    <row r="47" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D47" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47" s="51"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="68"/>
-      <c r="H47" s="70">
-        <v>19300</v>
-      </c>
-      <c r="I47" s="68"/>
-      <c r="J47" s="51"/>
-    </row>
-    <row r="48" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D48" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="E48" s="52"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="68"/>
-      <c r="H48" s="69">
-        <v>26400</v>
-      </c>
-      <c r="I48" s="51"/>
-      <c r="J48" s="52"/>
-    </row>
-    <row r="49" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D49" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="E49" s="51"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="68"/>
-      <c r="H49" s="70">
-        <v>15469</v>
-      </c>
-      <c r="I49" s="68"/>
-      <c r="J49" s="51"/>
-    </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D50" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="E50" s="51">
-        <v>60</v>
-      </c>
-      <c r="F50" s="49"/>
-      <c r="G50" s="68">
-        <v>35</v>
-      </c>
-      <c r="H50" s="69">
-        <v>31900</v>
-      </c>
-      <c r="I50" s="68">
-        <v>78</v>
-      </c>
-      <c r="J50" s="51">
-        <v>75.900000000000006</v>
-      </c>
-    </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D51" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" s="49"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="69">
-        <v>29100</v>
-      </c>
-      <c r="I51" s="49"/>
-      <c r="J51" s="49"/>
-    </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D52" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
-      <c r="G52" s="68"/>
-      <c r="H52" s="69">
-        <v>36100</v>
-      </c>
-      <c r="I52" s="49"/>
-      <c r="J52" s="49"/>
-    </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D53" s="49"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="49"/>
-      <c r="H53" s="49"/>
-      <c r="I53" s="49"/>
-      <c r="J53" s="49"/>
+      <c r="E65" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="F65" s="50"/>
+      <c r="G65" s="51">
+        <v>-0.75</v>
+      </c>
+      <c r="H65" s="51">
+        <v>1.9199999999999998E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>